<commit_message>
update to be ready in shiny-statics
</commit_message>
<xml_diff>
--- a/report/efa.xlsx
+++ b/report/efa.xlsx
@@ -12,12 +12,13 @@
     <sheet name="EFA-f5" r:id="rId6" sheetId="4"/>
     <sheet name="EFA-f4" r:id="rId7" sheetId="5"/>
     <sheet name="EFA-final" r:id="rId8" sheetId="6"/>
+    <sheet name="EFA-final-alt" r:id="rId9" sheetId="7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="141">
   <si>
     <t>Multivariate Normality Tests</t>
   </si>
@@ -457,7 +458,7 @@
 </t>
   </si>
   <si>
-    <t>Exploratory Factor Analysis EFA with n=3 factors (Final)</t>
+    <t>Exploratory Factor Analysis EFA with n=3 factors</t>
   </si>
   <si>
     <t xml:space="preserve">Mean item complexity = 1.26889748776893
@@ -471,13 +472,28 @@
 BIC = -177.284477317792
 </t>
   </si>
+  <si>
+    <t>Exploratory Factor Analysis Alternative EFA with n=3 factors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean item complexity = 1.17409070887675
+The degrees of freedom for the model are = 42
+The objective function was = 0.426582512916918
+The Chi Square of the model is = 107.887316779403
+The root mean square of the residuals (RMSR) is = 0.0426610066000907
+Tucker Lewis Index of factoring reliability is =  0.901885178102094
+RMSEA index =  0.0854395900327584
+The 90% confidence intervals of RMSEA are lower = 0.0716646306244335 and upper = 0.0999634220637349
+BIC = -90.8695948946509
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="360">
+  <fonts count="415">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -2242,6 +2258,367 @@
       <name val="Calibri"/>
       <sz val="12.0"/>
       <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -2770,7 +3147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="642">
+  <cellXfs count="751">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -3507,6 +3884,133 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="359" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="359" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="justify" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="360" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="361" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="362" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="363" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="364" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="365" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="366" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="367" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="368" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="369" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="370" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="371" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="372" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="373" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="373" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="373" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="374" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="375" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="376" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="377" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="378" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="379" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="380" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="381" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="382" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="383" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="384" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="384" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="384" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="385" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="386" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="387" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="388" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="389" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="390" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="391" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="392" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="393" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="394" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="395" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="395" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="395" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="396" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="397" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="398" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="399" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="400" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="401" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="402" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="403" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="404" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="405" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="406" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="406" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="406" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="407" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="408" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="409" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="410" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="411" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="412" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="413" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="414" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="414" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="justify" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -10134,4 +10638,576 @@
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="14.0" customWidth="true"/>
+    <col min="2" max="2" width="14.0" customWidth="true"/>
+    <col min="3" max="3" width="14.0" customWidth="true"/>
+    <col min="4" max="4" width="14.0" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="643">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="657">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5"/>
+      <c r="B5" t="s" s="671">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s" s="671">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s" s="671">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="667">
+        <v>81</v>
+      </c>
+      <c r="B6" t="n" s="672">
+        <v>-0.038</v>
+      </c>
+      <c r="C6" t="n" s="673">
+        <v>0.8356</v>
+      </c>
+      <c r="D6" t="n" s="674">
+        <v>-0.0612</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="667">
+        <v>82</v>
+      </c>
+      <c r="B7" t="n" s="672">
+        <v>-0.1972</v>
+      </c>
+      <c r="C7" t="n" s="673">
+        <v>0.8973</v>
+      </c>
+      <c r="D7" t="n" s="674">
+        <v>0.1486</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="667">
+        <v>83</v>
+      </c>
+      <c r="B8" t="n" s="672">
+        <v>0.0925</v>
+      </c>
+      <c r="C8" t="n" s="673">
+        <v>0.7538</v>
+      </c>
+      <c r="D8" t="n" s="674">
+        <v>-0.0344</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="667">
+        <v>84</v>
+      </c>
+      <c r="B9" t="n" s="672">
+        <v>0.314</v>
+      </c>
+      <c r="C9" t="n" s="673">
+        <v>0.5791</v>
+      </c>
+      <c r="D9" t="n" s="674">
+        <v>-0.0743</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="667">
+        <v>90</v>
+      </c>
+      <c r="B10" t="n" s="672">
+        <v>0.4548</v>
+      </c>
+      <c r="C10" t="n" s="673">
+        <v>-0.0238</v>
+      </c>
+      <c r="D10" t="n" s="674">
+        <v>0.0538</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="667">
+        <v>91</v>
+      </c>
+      <c r="B11" t="n" s="672">
+        <v>0.9056</v>
+      </c>
+      <c r="C11" t="n" s="673">
+        <v>0.0387</v>
+      </c>
+      <c r="D11" t="n" s="674">
+        <v>-0.1693</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="667">
+        <v>92</v>
+      </c>
+      <c r="B12" t="n" s="672">
+        <v>0.5068</v>
+      </c>
+      <c r="C12" t="n" s="673">
+        <v>-0.0117</v>
+      </c>
+      <c r="D12" t="n" s="674">
+        <v>0.0761</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="667">
+        <v>93</v>
+      </c>
+      <c r="B13" t="n" s="672">
+        <v>0.8842</v>
+      </c>
+      <c r="C13" t="n" s="673">
+        <v>-0.0926</v>
+      </c>
+      <c r="D13" t="n" s="674">
+        <v>-0.069</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="667">
+        <v>95</v>
+      </c>
+      <c r="B14" t="n" s="672">
+        <v>0.6217</v>
+      </c>
+      <c r="C14" t="n" s="673">
+        <v>0.0048</v>
+      </c>
+      <c r="D14" t="n" s="674">
+        <v>0.1145</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="667">
+        <v>96</v>
+      </c>
+      <c r="B15" t="n" s="672">
+        <v>0.5713</v>
+      </c>
+      <c r="C15" t="n" s="673">
+        <v>0.1115</v>
+      </c>
+      <c r="D15" t="n" s="674">
+        <v>0.0924</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="667">
+        <v>97</v>
+      </c>
+      <c r="B16" t="n" s="672">
+        <v>0.026</v>
+      </c>
+      <c r="C16" t="n" s="673">
+        <v>0.0203</v>
+      </c>
+      <c r="D16" t="n" s="674">
+        <v>0.7114</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="667">
+        <v>99</v>
+      </c>
+      <c r="B17" t="n" s="672">
+        <v>-0.0458</v>
+      </c>
+      <c r="C17" t="n" s="673">
+        <v>-0.0432</v>
+      </c>
+      <c r="D17" t="n" s="674">
+        <v>0.813</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="667">
+        <v>101</v>
+      </c>
+      <c r="B18" t="n" s="672">
+        <v>0.2154</v>
+      </c>
+      <c r="C18" t="n" s="673">
+        <v>0.129</v>
+      </c>
+      <c r="D18" t="n" s="674">
+        <v>0.3282</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="678">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22"/>
+      <c r="B22" t="s" s="692">
+        <v>110</v>
+      </c>
+      <c r="C22" t="s" s="692">
+        <v>115</v>
+      </c>
+      <c r="D22" t="s" s="692">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="688">
+        <v>110</v>
+      </c>
+      <c r="B23" t="n" s="693">
+        <v>1.0</v>
+      </c>
+      <c r="C23" t="n" s="694">
+        <v>0.7419</v>
+      </c>
+      <c r="D23" t="n" s="695">
+        <v>0.7815</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="688">
+        <v>115</v>
+      </c>
+      <c r="B24" t="n" s="693">
+        <v>0.7419</v>
+      </c>
+      <c r="C24" t="n" s="694">
+        <v>1.0</v>
+      </c>
+      <c r="D24" t="n" s="695">
+        <v>0.7347</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="688">
+        <v>112</v>
+      </c>
+      <c r="B25" t="n" s="693">
+        <v>0.7815</v>
+      </c>
+      <c r="C25" t="n" s="694">
+        <v>0.7347</v>
+      </c>
+      <c r="D25" t="n" s="695">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="699">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29"/>
+      <c r="B29" t="s" s="713">
+        <v>118</v>
+      </c>
+      <c r="C29" t="s" s="713">
+        <v>123</v>
+      </c>
+      <c r="D29" t="s" s="713">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="709">
+        <v>124</v>
+      </c>
+      <c r="B30" t="n" s="714">
+        <v>3.0067</v>
+      </c>
+      <c r="C30" t="n" s="715">
+        <v>2.5279</v>
+      </c>
+      <c r="D30" t="n" s="716">
+        <v>1.3785</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="709">
+        <v>125</v>
+      </c>
+      <c r="B31" t="n" s="714">
+        <v>0.2313</v>
+      </c>
+      <c r="C31" t="n" s="715">
+        <v>0.1945</v>
+      </c>
+      <c r="D31" t="n" s="716">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="709">
+        <v>126</v>
+      </c>
+      <c r="B32" t="n" s="714">
+        <v>0.2313</v>
+      </c>
+      <c r="C32" t="n" s="715">
+        <v>0.4257</v>
+      </c>
+      <c r="D32" t="n" s="716">
+        <v>0.5318</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="709">
+        <v>127</v>
+      </c>
+      <c r="B33" t="n" s="714">
+        <v>0.4349</v>
+      </c>
+      <c r="C33" t="n" s="715">
+        <v>0.3657</v>
+      </c>
+      <c r="D33" t="n" s="716">
+        <v>0.1994</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="709">
+        <v>128</v>
+      </c>
+      <c r="B34" t="n" s="714">
+        <v>0.4349</v>
+      </c>
+      <c r="C34" t="n" s="715">
+        <v>0.8006</v>
+      </c>
+      <c r="D34" t="n" s="716">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="720">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38"/>
+      <c r="B38" t="s" s="734">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="730">
+        <v>81</v>
+      </c>
+      <c r="B39" t="n" s="735">
+        <v>1.0149</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="730">
+        <v>82</v>
+      </c>
+      <c r="B40" t="n" s="735">
+        <v>1.1536</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="730">
+        <v>83</v>
+      </c>
+      <c r="B41" t="n" s="735">
+        <v>1.0343</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="730">
+        <v>84</v>
+      </c>
+      <c r="B42" t="n" s="735">
+        <v>1.5804</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="730">
+        <v>90</v>
+      </c>
+      <c r="B43" t="n" s="735">
+        <v>1.0335</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="730">
+        <v>91</v>
+      </c>
+      <c r="B44" t="n" s="735">
+        <v>1.0736</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="730">
+        <v>92</v>
+      </c>
+      <c r="B45" t="n" s="735">
+        <v>1.0462</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="730">
+        <v>93</v>
+      </c>
+      <c r="B46" t="n" s="735">
+        <v>1.0343</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="730">
+        <v>95</v>
+      </c>
+      <c r="B47" t="n" s="735">
+        <v>1.0679</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="730">
+        <v>96</v>
+      </c>
+      <c r="B48" t="n" s="735">
+        <v>1.1301</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="730">
+        <v>97</v>
+      </c>
+      <c r="B49" t="n" s="735">
+        <v>1.0043</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="730">
+        <v>99</v>
+      </c>
+      <c r="B50" t="n" s="735">
+        <v>1.012</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="730">
+        <v>101</v>
+      </c>
+      <c r="B51" t="n" s="735">
+        <v>2.078</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="739">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="750">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="A55:J59"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>